<commit_message>
change the demand data
</commit_message>
<xml_diff>
--- a/data/correlation/vessel_price_calc.xlsx
+++ b/data/correlation/vessel_price_calc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yoshinoriokubo/Documents/simulator/data/correlation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7306D28A-CD6A-4E4F-9A39-73F3BA7E1DB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78692E21-3D3D-924F-B938-329A3D48B06D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15860" activeTab="1" xr2:uid="{9983F2E6-F990-774E-B2F7-66EDAC9AA127}"/>
   </bookViews>
@@ -9584,8 +9584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5140633F-E656-3042-AF5A-0F03D3CDFEC7}">
   <dimension ref="A1:AA186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50:E149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>

</xml_diff>